<commit_message>
🧹 MAJOR CLEANUP: Organize project structure and archive test files
</commit_message>
<xml_diff>
--- a/dividend_stocks.xlsx
+++ b/dividend_stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjmat\Python Code in VS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D229746-F4CA-457A-B9EA-02B0D714CD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C400CA7-6925-4538-A241-4F064EA962C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Ticker</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Beginning Dividend Yield</t>
+  </si>
+  <si>
+    <t>08-16-2025</t>
   </si>
   <si>
     <t>08-09-2025</t>
@@ -280,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="51">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -555,6 +558,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -599,7 +614,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -698,6 +713,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1097,11 +1114,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL25"/>
+  <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S28" sqref="S28"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1133,7 @@
     <col min="16" max="16" width="12.85546875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1236,7 @@
       <c r="AH1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="28" t="s">
+      <c r="AI1" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="28" t="s">
@@ -1228,13 +1245,16 @@
       <c r="AK1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="75" t="s">
+      <c r="AL1" s="28" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" s="75" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="25">
         <v>1050</v>
@@ -1243,7 +1263,7 @@
         <v>13.877599999999999</v>
       </c>
       <c r="D2" s="21">
-        <v>11.82</v>
+        <v>11.6</v>
       </c>
       <c r="E2" s="1">
         <v>-108.24</v>
@@ -1256,7 +1276,7 @@
       </c>
       <c r="H2" s="9">
         <f t="shared" ref="H2:H23" si="0">B2*D2</f>
-        <v>12411</v>
+        <v>12180</v>
       </c>
       <c r="I2" s="16">
         <f t="shared" ref="I2:I23" si="1">B2*C2</f>
@@ -1264,99 +1284,102 @@
       </c>
       <c r="J2" s="9">
         <f t="shared" ref="J2:J23" si="2">H2-I2</f>
-        <v>-2160.4799999999996</v>
+        <v>-2391.4799999999996</v>
       </c>
       <c r="K2" s="33">
-        <v>45898.66065972222</v>
+        <v>45898.335150462961</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M2" s="8">
         <f t="shared" ref="M2:M19" si="3">((D2*Q2)/100)/12</f>
-        <v>0.10046999999999999</v>
+        <v>9.9856666666666663E-2</v>
       </c>
       <c r="N2" s="8">
         <f>(($B2*$D2)*(P2/100)/12)</f>
-        <v>146.86349999999999</v>
+        <v>144.13</v>
       </c>
       <c r="O2" s="8">
         <f>(($B2*$D2)*(Q2/100)/12)</f>
-        <v>105.4935</v>
+        <v>104.84949999999999</v>
       </c>
       <c r="P2" s="22">
         <v>14.2</v>
       </c>
-      <c r="Q2" s="76">
+      <c r="Q2" s="78">
+        <v>10.33</v>
+      </c>
+      <c r="R2" s="76">
         <v>10.199999999999999</v>
       </c>
-      <c r="R2" s="72">
+      <c r="S2" s="72">
         <v>10.75</v>
       </c>
-      <c r="S2" s="69">
+      <c r="T2" s="69">
         <v>9.93</v>
       </c>
-      <c r="T2" s="66">
+      <c r="U2" s="66">
         <v>10.57</v>
       </c>
-      <c r="U2" s="64">
+      <c r="V2" s="64">
         <v>10.67</v>
       </c>
-      <c r="V2" s="59">
+      <c r="W2" s="59">
         <v>10.85</v>
       </c>
-      <c r="W2" s="57">
+      <c r="X2" s="57">
         <v>11.17</v>
       </c>
-      <c r="X2" s="55">
+      <c r="Y2" s="55">
         <v>11.73</v>
       </c>
-      <c r="Y2" s="53">
+      <c r="Z2" s="53">
         <v>11.4</v>
       </c>
-      <c r="Z2" s="51">
+      <c r="AA2" s="51">
         <v>12.11</v>
       </c>
-      <c r="AA2" s="49">
+      <c r="AB2" s="49">
         <v>12.7</v>
       </c>
-      <c r="AB2" s="46">
+      <c r="AC2" s="46">
         <v>13.45</v>
       </c>
-      <c r="AC2" s="44">
+      <c r="AD2" s="44">
         <v>11.55</v>
       </c>
-      <c r="AD2" s="42">
+      <c r="AE2" s="42">
         <v>10.83</v>
       </c>
-      <c r="AE2" s="40">
+      <c r="AF2" s="40">
         <v>15.4</v>
       </c>
-      <c r="AF2" s="38">
+      <c r="AG2" s="38">
         <v>16.03</v>
       </c>
-      <c r="AG2" s="36">
+      <c r="AH2" s="36">
         <v>16.48</v>
       </c>
-      <c r="AH2" s="31">
+      <c r="AI2" s="31">
         <v>14.68</v>
       </c>
-      <c r="AI2" s="26">
+      <c r="AJ2" s="26">
         <v>14.63</v>
       </c>
-      <c r="AJ2" s="18">
+      <c r="AK2" s="18">
         <v>14.02</v>
       </c>
-      <c r="AK2" s="14">
+      <c r="AL2" s="14">
         <v>13.86</v>
       </c>
-      <c r="AL2" s="10" t="s">
-        <v>40</v>
+      <c r="AM2" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="25">
         <v>1625</v>
@@ -1365,7 +1388,7 @@
         <v>6.6412000000000004</v>
       </c>
       <c r="D3" s="21">
-        <v>5.95</v>
+        <v>5.94</v>
       </c>
       <c r="E3" s="1">
         <v>-32.5</v>
@@ -1378,7 +1401,7 @@
       </c>
       <c r="H3" s="9">
         <f t="shared" si="0"/>
-        <v>9668.75</v>
+        <v>9652.5</v>
       </c>
       <c r="I3" s="16">
         <f t="shared" si="1"/>
@@ -1386,99 +1409,102 @@
       </c>
       <c r="J3" s="9">
         <f t="shared" si="2"/>
-        <v>-1123.2000000000007</v>
+        <v>-1139.4500000000007</v>
       </c>
       <c r="K3" s="33">
-        <v>45869.66065972222</v>
+        <v>45898.335162037038</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M3" s="8">
         <f t="shared" si="3"/>
-        <v>7.7498750000000005E-2</v>
+        <v>7.6972499999999999E-2</v>
       </c>
       <c r="N3" s="8">
         <f t="shared" ref="N3:N23" si="4">((B3*D3)*(P3/100)/12)</f>
-        <v>125.12973958333333</v>
+        <v>124.9194375</v>
       </c>
       <c r="O3" s="8">
         <f t="shared" ref="O3:O23" si="5">(($B3*$D3)*(Q3/100)/12)</f>
-        <v>125.93546875</v>
+        <v>125.08031249999999</v>
       </c>
       <c r="P3" s="22">
         <v>15.53</v>
       </c>
-      <c r="Q3" s="77">
+      <c r="Q3" s="79">
+        <v>15.55</v>
+      </c>
+      <c r="R3" s="77">
         <v>15.63</v>
       </c>
-      <c r="R3" s="73">
+      <c r="S3" s="73">
         <v>15.63</v>
       </c>
-      <c r="S3" s="70">
+      <c r="T3" s="70">
         <v>15.63</v>
       </c>
-      <c r="T3" s="67">
+      <c r="U3" s="67">
         <v>15.6</v>
       </c>
-      <c r="U3" s="65">
+      <c r="V3" s="65">
         <v>15.58</v>
       </c>
-      <c r="V3" s="60">
+      <c r="W3" s="60">
         <v>15.66</v>
       </c>
-      <c r="W3" s="58">
+      <c r="X3" s="58">
         <v>15.87</v>
       </c>
-      <c r="X3" s="56">
+      <c r="Y3" s="56">
         <v>15.82</v>
       </c>
-      <c r="Y3" s="54">
+      <c r="Z3" s="54">
         <v>15.76</v>
       </c>
-      <c r="Z3" s="52">
+      <c r="AA3" s="52">
         <v>15.92</v>
       </c>
-      <c r="AA3" s="50">
+      <c r="AB3" s="50">
         <v>15.9</v>
       </c>
-      <c r="AB3" s="47">
+      <c r="AC3" s="47">
         <v>16.23</v>
       </c>
-      <c r="AC3" s="45">
+      <c r="AD3" s="45">
         <v>16.29</v>
       </c>
-      <c r="AD3" s="43">
+      <c r="AE3" s="43">
         <v>16.399999999999999</v>
       </c>
-      <c r="AE3" s="40">
+      <c r="AF3" s="40">
         <v>16.79</v>
       </c>
-      <c r="AF3" s="38">
+      <c r="AG3" s="38">
         <v>16.88</v>
       </c>
-      <c r="AG3" s="36">
+      <c r="AH3" s="36">
         <v>17.350000000000001</v>
       </c>
-      <c r="AH3" s="31">
+      <c r="AI3" s="31">
         <v>16.059999999999999</v>
       </c>
-      <c r="AI3" s="26">
+      <c r="AJ3" s="26">
         <v>15.74</v>
       </c>
-      <c r="AJ3" s="18">
+      <c r="AK3" s="18">
         <v>15.5</v>
       </c>
-      <c r="AK3" s="15">
+      <c r="AL3" s="15">
         <v>15.68</v>
       </c>
-      <c r="AL3" s="10" t="s">
-        <v>40</v>
+      <c r="AM3" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="25">
         <v>736</v>
@@ -1487,7 +1513,7 @@
         <v>10.37</v>
       </c>
       <c r="D4" s="21">
-        <v>9.4499999999999993</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="E4" s="1">
         <v>-51.52</v>
@@ -1500,7 +1526,7 @@
       </c>
       <c r="H4" s="9">
         <f t="shared" si="0"/>
-        <v>6955.2</v>
+        <v>7087.68</v>
       </c>
       <c r="I4" s="16">
         <f t="shared" si="1"/>
@@ -1508,99 +1534,102 @@
       </c>
       <c r="J4" s="9">
         <f t="shared" si="2"/>
-        <v>-677.11999999999989</v>
+        <v>-544.63999999999942</v>
       </c>
       <c r="K4" s="33">
-        <v>45910.66065972222</v>
+        <v>45910.335162037038</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M4" s="8">
         <f t="shared" si="3"/>
-        <v>0.12048750000000001</v>
+        <v>0.12021450000000002</v>
       </c>
       <c r="N4" s="8">
         <f t="shared" si="4"/>
-        <v>80.042760000000001</v>
+        <v>81.567384000000004</v>
       </c>
       <c r="O4" s="8">
         <f t="shared" si="5"/>
-        <v>88.67880000000001</v>
+        <v>88.477872000000005</v>
       </c>
       <c r="P4" s="22">
         <v>13.81</v>
       </c>
-      <c r="Q4" s="77">
+      <c r="Q4" s="79">
+        <v>14.98</v>
+      </c>
+      <c r="R4" s="77">
         <v>15.3</v>
       </c>
-      <c r="R4" s="73">
+      <c r="S4" s="73">
         <v>15.27</v>
       </c>
-      <c r="S4" s="70">
+      <c r="T4" s="70">
         <v>14.83</v>
       </c>
-      <c r="T4" s="67">
+      <c r="U4" s="67">
         <v>15.52</v>
       </c>
-      <c r="U4" s="65">
+      <c r="V4" s="65">
         <v>15.24</v>
       </c>
-      <c r="V4" s="60">
+      <c r="W4" s="60">
         <v>15.29</v>
       </c>
-      <c r="W4" s="58">
+      <c r="X4" s="58">
         <v>15.45</v>
       </c>
-      <c r="X4" s="56">
+      <c r="Y4" s="56">
         <v>15.55</v>
       </c>
-      <c r="Y4" s="54">
+      <c r="Z4" s="54">
         <v>15.32</v>
       </c>
-      <c r="Z4" s="52">
+      <c r="AA4" s="52">
         <v>15.93</v>
       </c>
-      <c r="AA4" s="50">
+      <c r="AB4" s="50">
         <v>16.309999999999999</v>
       </c>
-      <c r="AB4" s="47">
+      <c r="AC4" s="47">
         <v>16.350000000000001</v>
       </c>
-      <c r="AC4" s="45">
+      <c r="AD4" s="45">
         <v>16.22</v>
       </c>
-      <c r="AD4" s="43">
+      <c r="AE4" s="43">
         <v>16.350000000000001</v>
       </c>
-      <c r="AE4" s="40">
+      <c r="AF4" s="40">
         <v>16.510000000000002</v>
       </c>
-      <c r="AF4" s="38">
+      <c r="AG4" s="38">
         <v>17.350000000000001</v>
       </c>
-      <c r="AG4" s="36">
+      <c r="AH4" s="36">
         <v>17.73</v>
       </c>
-      <c r="AH4" s="31">
+      <c r="AI4" s="31">
         <v>15.42</v>
       </c>
-      <c r="AI4" s="26">
+      <c r="AJ4" s="26">
         <v>15.13</v>
       </c>
-      <c r="AJ4" s="19">
+      <c r="AK4" s="19">
         <v>14.17</v>
       </c>
-      <c r="AK4" s="15">
+      <c r="AL4" s="15">
         <v>14.06</v>
       </c>
-      <c r="AL4" s="10" t="s">
-        <v>40</v>
+      <c r="AM4" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="25">
         <v>440</v>
@@ -1609,7 +1638,7 @@
         <v>28.001799999999999</v>
       </c>
       <c r="D5" s="21">
-        <v>21.09</v>
+        <v>21.17</v>
       </c>
       <c r="E5" s="1">
         <v>-118.8</v>
@@ -1622,7 +1651,7 @@
       </c>
       <c r="H5" s="9">
         <f t="shared" si="0"/>
-        <v>9279.6</v>
+        <v>9314.8000000000011</v>
       </c>
       <c r="I5" s="16">
         <f t="shared" si="1"/>
@@ -1630,99 +1659,102 @@
       </c>
       <c r="J5" s="9">
         <f t="shared" si="2"/>
-        <v>-3041.1919999999991</v>
+        <v>-3005.9919999999984</v>
       </c>
       <c r="K5" s="33">
-        <v>45876.660671296297</v>
+        <v>45876.335162037038</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M5" s="8">
         <f t="shared" si="3"/>
-        <v>0.9026519999999999</v>
+        <v>0.90342975000000003</v>
       </c>
       <c r="N5" s="8">
         <f t="shared" si="4"/>
-        <v>441.32231000000002</v>
+        <v>442.99636333333336</v>
       </c>
       <c r="O5" s="8">
         <f t="shared" si="5"/>
-        <v>397.16687999999999</v>
+        <v>397.50909000000001</v>
       </c>
       <c r="P5" s="22">
         <v>57.07</v>
       </c>
-      <c r="Q5" s="76">
+      <c r="Q5" s="78">
+        <v>51.21</v>
+      </c>
+      <c r="R5" s="76">
         <v>51.36</v>
       </c>
-      <c r="R5" s="72">
+      <c r="S5" s="72">
         <v>51.67</v>
       </c>
-      <c r="S5" s="69">
+      <c r="T5" s="69">
         <v>49.83</v>
       </c>
-      <c r="T5" s="66">
+      <c r="U5" s="66">
         <v>48.92</v>
       </c>
-      <c r="U5" s="64">
+      <c r="V5" s="64">
         <v>51.27</v>
       </c>
-      <c r="V5" s="59">
+      <c r="W5" s="59">
         <v>52.94</v>
       </c>
-      <c r="W5" s="57">
+      <c r="X5" s="57">
         <v>55.31</v>
       </c>
-      <c r="X5" s="56">
+      <c r="Y5" s="56">
         <v>57.33</v>
       </c>
-      <c r="Y5" s="53">
+      <c r="Z5" s="53">
         <v>55.67</v>
       </c>
-      <c r="Z5" s="52">
+      <c r="AA5" s="52">
         <v>58.32</v>
       </c>
-      <c r="AA5" s="49">
+      <c r="AB5" s="49">
         <v>56.87</v>
       </c>
-      <c r="AB5" s="46">
+      <c r="AC5" s="46">
         <v>54.14</v>
       </c>
-      <c r="AC5" s="45">
+      <c r="AD5" s="45">
         <v>59.28</v>
       </c>
-      <c r="AD5" s="43">
+      <c r="AE5" s="43">
         <v>62.12</v>
       </c>
-      <c r="AE5" s="40">
+      <c r="AF5" s="40">
         <v>67.78</v>
       </c>
-      <c r="AF5" s="38">
+      <c r="AG5" s="38">
         <v>75.319999999999993</v>
       </c>
-      <c r="AG5" s="36">
+      <c r="AH5" s="36">
         <v>79.84</v>
       </c>
-      <c r="AH5" s="31">
+      <c r="AI5" s="31">
         <v>77.52</v>
       </c>
-      <c r="AI5" s="26">
+      <c r="AJ5" s="26">
         <v>74.83</v>
       </c>
-      <c r="AJ5" s="19">
+      <c r="AK5" s="19">
         <v>74.83</v>
       </c>
-      <c r="AK5" s="15">
+      <c r="AL5" s="15">
         <v>74.83</v>
       </c>
-      <c r="AL5" s="10" t="s">
-        <v>40</v>
+      <c r="AM5" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="25">
         <v>568</v>
@@ -1731,7 +1763,7 @@
         <v>5.7</v>
       </c>
       <c r="D6" s="21">
-        <v>5.33</v>
+        <v>5.54</v>
       </c>
       <c r="E6" s="1">
         <v>-28.4</v>
@@ -1744,7 +1776,7 @@
       </c>
       <c r="H6" s="9">
         <f t="shared" si="0"/>
-        <v>3027.44</v>
+        <v>3146.72</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" si="1"/>
@@ -1752,99 +1784,102 @@
       </c>
       <c r="J6" s="9">
         <f t="shared" si="2"/>
-        <v>-210.15999999999985</v>
+        <v>-90.880000000000109</v>
       </c>
       <c r="K6" s="33">
-        <v>45852.660671296297</v>
+        <v>45852.335162037038</v>
       </c>
       <c r="L6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M6" s="8">
         <f t="shared" si="3"/>
-        <v>5.321116666666667E-2</v>
+        <v>5.3045500000000002E-2</v>
       </c>
       <c r="N6" s="8">
         <f t="shared" si="4"/>
-        <v>26.010755333333336</v>
+        <v>27.035569333333331</v>
       </c>
       <c r="O6" s="8">
         <f t="shared" si="5"/>
-        <v>30.22394266666667</v>
+        <v>30.129844000000002</v>
       </c>
       <c r="P6" s="22">
         <v>10.31</v>
       </c>
-      <c r="Q6" s="77">
+      <c r="Q6" s="79">
+        <v>11.49</v>
+      </c>
+      <c r="R6" s="77">
         <v>11.98</v>
       </c>
-      <c r="R6" s="73">
+      <c r="S6" s="73">
         <v>12.36</v>
       </c>
-      <c r="S6" s="70">
+      <c r="T6" s="70">
         <v>13.03</v>
       </c>
-      <c r="T6" s="67">
+      <c r="U6" s="67">
         <v>12.88</v>
       </c>
-      <c r="U6" s="65">
+      <c r="V6" s="65">
         <v>12.55</v>
       </c>
-      <c r="V6" s="60">
+      <c r="W6" s="60">
         <v>12.24</v>
       </c>
-      <c r="W6" s="58">
+      <c r="X6" s="58">
         <v>12.17</v>
       </c>
-      <c r="X6" s="56">
+      <c r="Y6" s="56">
         <v>12.5</v>
       </c>
-      <c r="Y6" s="54">
+      <c r="Z6" s="54">
         <v>11.96</v>
       </c>
-      <c r="Z6" s="52">
+      <c r="AA6" s="52">
         <v>12.6</v>
       </c>
-      <c r="AA6" s="50">
+      <c r="AB6" s="50">
         <v>12.7</v>
       </c>
-      <c r="AB6" s="47">
+      <c r="AC6" s="47">
         <v>12.6</v>
       </c>
-      <c r="AC6" s="45">
+      <c r="AD6" s="45">
         <v>12.28</v>
       </c>
-      <c r="AD6" s="43">
+      <c r="AE6" s="43">
         <v>12.77</v>
       </c>
-      <c r="AE6" s="40">
+      <c r="AF6" s="40">
         <v>13.53</v>
       </c>
-      <c r="AF6" s="38">
+      <c r="AG6" s="38">
         <v>14.48</v>
       </c>
-      <c r="AG6" s="36">
+      <c r="AH6" s="36">
         <v>14.41</v>
       </c>
-      <c r="AH6" s="31">
+      <c r="AI6" s="31">
         <v>11.83</v>
       </c>
-      <c r="AI6" s="26">
+      <c r="AJ6" s="26">
         <v>11.27</v>
       </c>
-      <c r="AJ6" s="19">
+      <c r="AK6" s="19">
         <v>10.77</v>
       </c>
-      <c r="AK6" s="15">
+      <c r="AL6" s="15">
         <v>10.65</v>
       </c>
-      <c r="AL6" s="10" t="s">
-        <v>40</v>
+      <c r="AM6" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7" s="25">
         <v>2425</v>
@@ -1853,7 +1888,7 @@
         <v>3.3992800000000001</v>
       </c>
       <c r="D7" s="21">
-        <v>2.85</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1">
         <v>-242.5</v>
@@ -1866,7 +1901,7 @@
       </c>
       <c r="H7" s="9">
         <f t="shared" si="0"/>
-        <v>6911.25</v>
+        <v>7275</v>
       </c>
       <c r="I7" s="16">
         <f t="shared" si="1"/>
@@ -1874,99 +1909,102 @@
       </c>
       <c r="J7" s="9">
         <f t="shared" si="2"/>
-        <v>-1332.0040000000008</v>
+        <v>-968.25400000000081</v>
       </c>
       <c r="K7" s="33">
-        <v>45869.660671296297</v>
+        <v>45869.335162037038</v>
       </c>
       <c r="L7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M7" s="8">
         <f t="shared" si="3"/>
-        <v>5.1086250000000007E-2</v>
+        <v>5.1025000000000008E-2</v>
       </c>
       <c r="N7" s="8">
         <f t="shared" si="4"/>
-        <v>97.909375000000011</v>
+        <v>103.0625</v>
       </c>
       <c r="O7" s="8">
         <f t="shared" si="5"/>
-        <v>123.88415625</v>
+        <v>123.73562500000001</v>
       </c>
       <c r="P7" s="22">
         <v>17</v>
       </c>
-      <c r="Q7" s="77">
+      <c r="Q7" s="79">
+        <v>20.41</v>
+      </c>
+      <c r="R7" s="77">
         <v>21.51</v>
       </c>
-      <c r="R7" s="73">
+      <c r="S7" s="73">
         <v>21.58</v>
       </c>
-      <c r="S7" s="70">
+      <c r="T7" s="70">
         <v>22.22</v>
       </c>
-      <c r="T7" s="67">
+      <c r="U7" s="67">
         <v>22.56</v>
       </c>
-      <c r="U7" s="65">
+      <c r="V7" s="65">
         <v>21.43</v>
       </c>
-      <c r="V7" s="60">
+      <c r="W7" s="60">
         <v>21.66</v>
       </c>
-      <c r="W7" s="58">
+      <c r="X7" s="58">
         <v>20.13</v>
       </c>
-      <c r="X7" s="56">
+      <c r="Y7" s="56">
         <v>20.55</v>
       </c>
-      <c r="Y7" s="54">
+      <c r="Z7" s="54">
         <v>20.13</v>
       </c>
-      <c r="Z7" s="52">
+      <c r="AA7" s="52">
         <v>20.2</v>
       </c>
-      <c r="AA7" s="50">
+      <c r="AB7" s="50">
         <v>20.34</v>
       </c>
-      <c r="AB7" s="47">
+      <c r="AC7" s="47">
         <v>20.13</v>
       </c>
-      <c r="AC7" s="45">
+      <c r="AD7" s="45">
         <v>19.8</v>
       </c>
-      <c r="AD7" s="43">
+      <c r="AE7" s="43">
         <v>20.34</v>
       </c>
-      <c r="AE7" s="40">
+      <c r="AF7" s="40">
         <v>22.39</v>
       </c>
-      <c r="AF7" s="38">
+      <c r="AG7" s="38">
         <v>22.39</v>
       </c>
-      <c r="AG7" s="36">
+      <c r="AH7" s="36">
         <v>24.49</v>
       </c>
-      <c r="AH7" s="31">
+      <c r="AI7" s="31">
         <v>19.29</v>
       </c>
-      <c r="AI7" s="26">
+      <c r="AJ7" s="26">
         <v>17.440000000000001</v>
       </c>
-      <c r="AJ7" s="18">
+      <c r="AK7" s="18">
         <v>16.670000000000002</v>
       </c>
-      <c r="AK7" s="14">
+      <c r="AL7" s="14">
         <v>16.670000000000002</v>
       </c>
-      <c r="AL7" s="10" t="s">
-        <v>40</v>
+      <c r="AM7" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="25">
         <v>260</v>
@@ -1975,7 +2013,7 @@
         <v>12.5</v>
       </c>
       <c r="D8" s="21">
-        <v>12.3</v>
+        <v>12.24</v>
       </c>
       <c r="E8" s="1">
         <v>5.2</v>
@@ -1988,7 +2026,7 @@
       </c>
       <c r="H8" s="9">
         <f t="shared" si="0"/>
-        <v>3198</v>
+        <v>3182.4</v>
       </c>
       <c r="I8" s="16">
         <f t="shared" si="1"/>
@@ -1996,99 +2034,102 @@
       </c>
       <c r="J8" s="9">
         <f t="shared" si="2"/>
-        <v>-52</v>
+        <v>-67.599999999999909</v>
       </c>
       <c r="K8" s="33">
-        <v>45898.660671296297</v>
+        <v>45898.335173611107</v>
       </c>
       <c r="L8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M8" s="8">
         <f t="shared" si="3"/>
-        <v>0.1110075</v>
+        <v>0.10985400000000001</v>
       </c>
       <c r="N8" s="8">
         <f t="shared" si="4"/>
-        <v>33.978749999999998</v>
+        <v>33.813000000000002</v>
       </c>
       <c r="O8" s="8">
         <f t="shared" si="5"/>
-        <v>28.861950000000004</v>
+        <v>28.562039999999996</v>
       </c>
       <c r="P8" s="22">
         <v>12.75</v>
       </c>
-      <c r="Q8" s="76">
+      <c r="Q8" s="78">
+        <v>10.77</v>
+      </c>
+      <c r="R8" s="76">
         <v>10.83</v>
       </c>
-      <c r="R8" s="72">
+      <c r="S8" s="72">
         <v>10.86</v>
       </c>
-      <c r="S8" s="69">
+      <c r="T8" s="69">
         <v>10.97</v>
       </c>
-      <c r="T8" s="66">
+      <c r="U8" s="66">
         <v>10.97</v>
       </c>
-      <c r="U8" s="64">
+      <c r="V8" s="64">
         <v>10.86</v>
       </c>
-      <c r="V8" s="59">
+      <c r="W8" s="59">
         <v>10.78</v>
       </c>
-      <c r="W8" s="57">
+      <c r="X8" s="57">
         <v>10.78</v>
       </c>
-      <c r="X8" s="55">
+      <c r="Y8" s="55">
         <v>10.95</v>
       </c>
-      <c r="Y8" s="53">
+      <c r="Z8" s="53">
         <v>10.71</v>
       </c>
-      <c r="Z8" s="51">
+      <c r="AA8" s="51">
         <v>10.73</v>
       </c>
-      <c r="AA8" s="49">
+      <c r="AB8" s="49">
         <v>10.78</v>
       </c>
-      <c r="AB8" s="46">
+      <c r="AC8" s="46">
         <v>10.99</v>
       </c>
-      <c r="AC8" s="44">
+      <c r="AD8" s="44">
         <v>10.91</v>
       </c>
-      <c r="AD8" s="42">
+      <c r="AE8" s="42">
         <v>10.95</v>
       </c>
-      <c r="AE8" s="41">
+      <c r="AF8" s="41">
         <v>11.15</v>
       </c>
-      <c r="AF8" s="39">
+      <c r="AG8" s="39">
         <v>11.38</v>
       </c>
-      <c r="AG8" s="37">
+      <c r="AH8" s="37">
         <v>11.71</v>
       </c>
-      <c r="AH8" s="32">
+      <c r="AI8" s="32">
         <v>10.69</v>
       </c>
-      <c r="AI8" s="26">
+      <c r="AJ8" s="26">
         <v>12.75</v>
       </c>
-      <c r="AJ8" s="19">
+      <c r="AK8" s="19">
         <v>12.75</v>
       </c>
-      <c r="AK8" s="15">
+      <c r="AL8" s="15">
         <v>12.75</v>
       </c>
-      <c r="AL8" s="10" t="s">
-        <v>40</v>
+      <c r="AM8" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="25">
         <v>625</v>
@@ -2097,7 +2138,7 @@
         <v>11.9018</v>
       </c>
       <c r="D9" s="21">
-        <v>12.42</v>
+        <v>12.58</v>
       </c>
       <c r="E9" s="1">
         <v>-37.94</v>
@@ -2110,7 +2151,7 @@
       </c>
       <c r="H9" s="9">
         <f t="shared" si="0"/>
-        <v>7762.5</v>
+        <v>7862.5</v>
       </c>
       <c r="I9" s="16">
         <f t="shared" si="1"/>
@@ -2118,99 +2159,102 @@
       </c>
       <c r="J9" s="9">
         <f t="shared" si="2"/>
-        <v>323.875</v>
+        <v>423.875</v>
       </c>
       <c r="K9" s="33">
-        <v>45870.660671296297</v>
+        <v>45902.335173611107</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M9" s="8">
         <f t="shared" si="3"/>
-        <v>0.17129249999999999</v>
+        <v>0.1701445</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" si="4"/>
-        <v>94.573125000000005</v>
+        <v>95.791458333333324</v>
       </c>
       <c r="O9" s="8">
         <f t="shared" si="5"/>
-        <v>107.05781250000001</v>
+        <v>106.3403125</v>
       </c>
       <c r="P9" s="22">
         <v>14.62</v>
       </c>
-      <c r="Q9" s="77">
+      <c r="Q9" s="79">
+        <v>16.23</v>
+      </c>
+      <c r="R9" s="77">
         <v>16.55</v>
       </c>
-      <c r="R9" s="73">
+      <c r="S9" s="73">
         <v>16.399999999999999</v>
       </c>
-      <c r="S9" s="70">
+      <c r="T9" s="70">
         <v>16</v>
       </c>
-      <c r="T9" s="67">
+      <c r="U9" s="67">
         <v>16.22</v>
       </c>
-      <c r="U9" s="65">
+      <c r="V9" s="65">
         <v>15.89</v>
       </c>
-      <c r="V9" s="60">
+      <c r="W9" s="60">
         <v>16.25</v>
       </c>
-      <c r="W9" s="58">
+      <c r="X9" s="58">
         <v>16.72</v>
       </c>
-      <c r="X9" s="56">
+      <c r="Y9" s="56">
         <v>16.71</v>
       </c>
-      <c r="Y9" s="54">
+      <c r="Z9" s="54">
         <v>16.45</v>
       </c>
-      <c r="Z9" s="52">
+      <c r="AA9" s="52">
         <v>16.86</v>
       </c>
-      <c r="AA9" s="50">
+      <c r="AB9" s="50">
         <v>17.16</v>
       </c>
-      <c r="AB9" s="47">
+      <c r="AC9" s="47">
         <v>17.260000000000002</v>
       </c>
-      <c r="AC9" s="45">
+      <c r="AD9" s="45">
         <v>16.43</v>
       </c>
-      <c r="AD9" s="43">
+      <c r="AE9" s="43">
         <v>16.73</v>
       </c>
-      <c r="AE9" s="40">
+      <c r="AF9" s="40">
         <v>17.03</v>
       </c>
-      <c r="AF9" s="38">
+      <c r="AG9" s="38">
         <v>17.600000000000001</v>
       </c>
-      <c r="AG9" s="36">
+      <c r="AH9" s="36">
         <v>18.329999999999998</v>
       </c>
-      <c r="AH9" s="31">
+      <c r="AI9" s="31">
         <v>16.059999999999999</v>
       </c>
-      <c r="AI9" s="26">
+      <c r="AJ9" s="26">
         <v>15.63</v>
       </c>
-      <c r="AJ9" s="18">
+      <c r="AK9" s="18">
         <v>14.53</v>
       </c>
-      <c r="AK9" s="14">
+      <c r="AL9" s="14">
         <v>14.35</v>
       </c>
-      <c r="AL9" s="10" t="s">
-        <v>40</v>
+      <c r="AM9" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" s="25">
         <v>1142</v>
@@ -2219,7 +2263,7 @@
         <v>10.0969</v>
       </c>
       <c r="D10" s="21">
-        <v>6.23</v>
+        <v>6.71</v>
       </c>
       <c r="E10" s="1">
         <v>30.36</v>
@@ -2232,7 +2276,7 @@
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>7114.6600000000008</v>
+        <v>7662.82</v>
       </c>
       <c r="I10" s="16">
         <f t="shared" si="1"/>
@@ -2240,99 +2284,102 @@
       </c>
       <c r="J10" s="9">
         <f t="shared" si="2"/>
-        <v>-4415.9997999999987</v>
+        <v>-3867.8397999999997</v>
       </c>
       <c r="K10" s="33">
-        <v>45898.660671296297</v>
+        <v>45930.335173611107</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M10" s="8">
         <f t="shared" si="3"/>
-        <v>0.13607358333333336</v>
+        <v>0.14107774999999997</v>
       </c>
       <c r="N10" s="8">
         <f t="shared" si="4"/>
-        <v>114.72389250000002</v>
+        <v>123.5629725</v>
       </c>
       <c r="O10" s="8">
         <f t="shared" si="5"/>
-        <v>155.39603216666669</v>
+        <v>161.11079050000001</v>
       </c>
       <c r="P10" s="22">
         <v>19.350000000000001</v>
       </c>
-      <c r="Q10" s="77">
+      <c r="Q10" s="79">
+        <v>25.23</v>
+      </c>
+      <c r="R10" s="77">
         <v>26.21</v>
       </c>
-      <c r="R10" s="73">
+      <c r="S10" s="73">
         <v>24.42</v>
       </c>
-      <c r="S10" s="70">
+      <c r="T10" s="70">
         <v>24.31</v>
       </c>
-      <c r="T10" s="67">
+      <c r="U10" s="67">
         <v>22.67</v>
       </c>
-      <c r="U10" s="65">
+      <c r="V10" s="65">
         <v>21.93</v>
       </c>
-      <c r="V10" s="60">
+      <c r="W10" s="60">
         <v>21.65</v>
       </c>
-      <c r="W10" s="58">
+      <c r="X10" s="58">
         <v>22.31</v>
       </c>
-      <c r="X10" s="56">
+      <c r="Y10" s="56">
         <v>22.31</v>
       </c>
-      <c r="Y10" s="54">
+      <c r="Z10" s="54">
         <v>22.16</v>
       </c>
-      <c r="Z10" s="52">
+      <c r="AA10" s="52">
         <v>21.65</v>
       </c>
-      <c r="AA10" s="50">
+      <c r="AB10" s="50">
         <v>21.37</v>
       </c>
-      <c r="AB10" s="47">
+      <c r="AC10" s="47">
         <v>22.58</v>
       </c>
-      <c r="AC10" s="45">
+      <c r="AD10" s="45">
         <v>21.03</v>
       </c>
-      <c r="AD10" s="43">
+      <c r="AE10" s="43">
         <v>21.62</v>
       </c>
-      <c r="AE10" s="40">
+      <c r="AF10" s="40">
         <v>21.76</v>
       </c>
-      <c r="AF10" s="38">
+      <c r="AG10" s="38">
         <v>23.05</v>
       </c>
-      <c r="AG10" s="36">
+      <c r="AH10" s="36">
         <v>23.08</v>
       </c>
-      <c r="AH10" s="31">
+      <c r="AI10" s="31">
         <v>21.71</v>
       </c>
-      <c r="AI10" s="26">
+      <c r="AJ10" s="26">
         <v>20.87</v>
       </c>
-      <c r="AJ10" s="19">
+      <c r="AK10" s="19">
         <v>21.21</v>
       </c>
-      <c r="AK10" s="15">
+      <c r="AL10" s="15">
         <v>20.39</v>
       </c>
-      <c r="AL10" s="10" t="s">
-        <v>40</v>
+      <c r="AM10" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="25">
         <v>466</v>
@@ -2341,7 +2388,7 @@
         <v>15.65</v>
       </c>
       <c r="D11" s="21">
-        <v>12.18</v>
+        <v>13.07</v>
       </c>
       <c r="E11" s="1">
         <v>-18.64</v>
@@ -2354,7 +2401,7 @@
       </c>
       <c r="H11" s="9">
         <f t="shared" si="0"/>
-        <v>5675.88</v>
+        <v>6090.62</v>
       </c>
       <c r="I11" s="16">
         <f t="shared" si="1"/>
@@ -2362,99 +2409,102 @@
       </c>
       <c r="J11" s="9">
         <f t="shared" si="2"/>
-        <v>-1617.0200000000004</v>
+        <v>-1202.2800000000007</v>
       </c>
       <c r="K11" s="33">
-        <v>45898.660682870373</v>
+        <v>45930.335173611107</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M11" s="8">
         <f t="shared" si="3"/>
-        <v>0.1292095</v>
+        <v>0.13080891666666666</v>
       </c>
       <c r="N11" s="8">
         <f t="shared" si="4"/>
-        <v>72.036377000000002</v>
+        <v>77.300118833333329</v>
       </c>
       <c r="O11" s="8">
         <f t="shared" si="5"/>
-        <v>60.211627</v>
+        <v>60.956955166666667</v>
       </c>
       <c r="P11" s="22">
         <v>15.23</v>
       </c>
-      <c r="Q11" s="76">
+      <c r="Q11" s="78">
+        <v>12.01</v>
+      </c>
+      <c r="R11" s="76">
         <v>12.73</v>
       </c>
-      <c r="R11" s="72">
+      <c r="S11" s="72">
         <v>12.01</v>
       </c>
-      <c r="S11" s="69">
+      <c r="T11" s="69">
         <v>12.05</v>
       </c>
-      <c r="T11" s="66">
+      <c r="U11" s="66">
         <v>11.61</v>
       </c>
-      <c r="U11" s="64">
+      <c r="V11" s="64">
         <v>11.24</v>
       </c>
-      <c r="V11" s="59">
+      <c r="W11" s="59">
         <v>11.35</v>
       </c>
-      <c r="W11" s="57">
+      <c r="X11" s="57">
         <v>11.62</v>
       </c>
-      <c r="X11" s="55">
+      <c r="Y11" s="55">
         <v>11.66</v>
       </c>
-      <c r="Y11" s="53">
+      <c r="Z11" s="53">
         <v>11.86</v>
       </c>
-      <c r="Z11" s="51">
+      <c r="AA11" s="51">
         <v>12.17</v>
       </c>
-      <c r="AA11" s="49">
+      <c r="AB11" s="49">
         <v>11.8</v>
       </c>
-      <c r="AB11" s="47">
+      <c r="AC11" s="47">
         <v>16.72</v>
       </c>
-      <c r="AC11" s="45">
+      <c r="AD11" s="45">
         <v>16.670000000000002</v>
       </c>
-      <c r="AD11" s="43">
+      <c r="AE11" s="43">
         <v>17.13</v>
       </c>
-      <c r="AE11" s="40">
+      <c r="AF11" s="40">
         <v>17.13</v>
       </c>
-      <c r="AF11" s="38">
+      <c r="AG11" s="38">
         <v>17.38</v>
       </c>
-      <c r="AG11" s="36">
+      <c r="AH11" s="36">
         <v>17.079999999999998</v>
       </c>
-      <c r="AH11" s="31">
+      <c r="AI11" s="31">
         <v>16.18</v>
       </c>
-      <c r="AI11" s="26">
+      <c r="AJ11" s="26">
         <v>16.02</v>
       </c>
-      <c r="AJ11" s="19">
+      <c r="AK11" s="19">
         <v>16.04</v>
       </c>
-      <c r="AK11" s="15">
+      <c r="AL11" s="15">
         <v>15.75</v>
       </c>
-      <c r="AL11" s="10" t="s">
-        <v>40</v>
+      <c r="AM11" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" s="25">
         <v>90</v>
@@ -2463,7 +2513,7 @@
         <v>11.3</v>
       </c>
       <c r="D12" s="21">
-        <v>10.61</v>
+        <v>10.73</v>
       </c>
       <c r="E12" s="1">
         <v>-18.899999999999999</v>
@@ -2476,7 +2526,7 @@
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>954.9</v>
+        <v>965.7</v>
       </c>
       <c r="I12" s="16">
         <f t="shared" si="1"/>
@@ -2484,99 +2534,102 @@
       </c>
       <c r="J12" s="9">
         <f t="shared" si="2"/>
-        <v>-62.100000000000136</v>
+        <v>-51.300000000000068</v>
       </c>
       <c r="K12" s="33">
-        <v>45845.660682870373</v>
+        <v>45845.335173611107</v>
       </c>
       <c r="L12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M12" s="8">
         <f t="shared" si="3"/>
-        <v>0.10981349999999999</v>
+        <v>0.10926716666666669</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" si="4"/>
-        <v>8.6179725000000005</v>
+        <v>8.7154425</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" si="5"/>
-        <v>9.8832149999999999</v>
+        <v>9.8340450000000015</v>
       </c>
       <c r="P12" s="22">
         <v>10.83</v>
       </c>
-      <c r="Q12" s="77">
+      <c r="Q12" s="79">
+        <v>12.22</v>
+      </c>
+      <c r="R12" s="77">
         <v>12.42</v>
       </c>
-      <c r="R12" s="73">
+      <c r="S12" s="73">
         <v>12.61</v>
       </c>
-      <c r="S12" s="70">
+      <c r="T12" s="70">
         <v>12.19</v>
       </c>
-      <c r="T12" s="67">
+      <c r="U12" s="67">
         <v>12.52</v>
       </c>
-      <c r="U12" s="65">
+      <c r="V12" s="65">
         <v>12.31</v>
       </c>
-      <c r="V12" s="60">
+      <c r="W12" s="60">
         <v>12.43</v>
       </c>
-      <c r="W12" s="58">
+      <c r="X12" s="58">
         <v>12.4</v>
       </c>
-      <c r="X12" s="56">
+      <c r="Y12" s="56">
         <v>12.61</v>
       </c>
-      <c r="Y12" s="54">
+      <c r="Z12" s="54">
         <v>12.38</v>
       </c>
-      <c r="Z12" s="52">
+      <c r="AA12" s="52">
         <v>12.76</v>
       </c>
-      <c r="AA12" s="50">
+      <c r="AB12" s="50">
         <v>13.02</v>
       </c>
-      <c r="AB12" s="47">
+      <c r="AC12" s="47">
         <v>13.05</v>
       </c>
-      <c r="AC12" s="45">
+      <c r="AD12" s="45">
         <v>12.76</v>
       </c>
-      <c r="AD12" s="43">
+      <c r="AE12" s="43">
         <v>12.78</v>
       </c>
-      <c r="AE12" s="40">
+      <c r="AF12" s="40">
         <v>13.17</v>
       </c>
-      <c r="AF12" s="38">
+      <c r="AG12" s="38">
         <v>13.88</v>
       </c>
-      <c r="AG12" s="36">
+      <c r="AH12" s="36">
         <v>14.2</v>
       </c>
-      <c r="AH12" s="31">
+      <c r="AI12" s="31">
         <v>12.43</v>
       </c>
-      <c r="AI12" s="27">
+      <c r="AJ12" s="27">
         <v>10.41</v>
       </c>
-      <c r="AJ12" s="19">
+      <c r="AK12" s="19">
         <v>10.83</v>
       </c>
-      <c r="AK12" s="15">
+      <c r="AL12" s="15">
         <v>10.83</v>
       </c>
-      <c r="AL12" s="10" t="s">
-        <v>40</v>
+      <c r="AM12" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B13" s="25">
         <v>917</v>
@@ -2585,7 +2638,7 @@
         <v>8.1135999999999999</v>
       </c>
       <c r="D13" s="21">
-        <v>7.41</v>
+        <v>7.37</v>
       </c>
       <c r="E13" s="1">
         <v>-82.53</v>
@@ -2598,7 +2651,7 @@
       </c>
       <c r="H13" s="9">
         <f t="shared" si="0"/>
-        <v>6794.97</v>
+        <v>6758.29</v>
       </c>
       <c r="I13" s="16">
         <f t="shared" si="1"/>
@@ -2606,99 +2659,102 @@
       </c>
       <c r="J13" s="9">
         <f t="shared" si="2"/>
-        <v>-645.20119999999952</v>
+        <v>-681.88119999999981</v>
       </c>
       <c r="K13" s="33">
-        <v>45898.660682870373</v>
+        <v>45898.335173611107</v>
       </c>
       <c r="L13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M13" s="8">
         <f t="shared" si="3"/>
-        <v>9.0340250000000011E-2</v>
+        <v>9.071241666666667E-2</v>
       </c>
       <c r="N13" s="8">
         <f t="shared" si="4"/>
-        <v>78.821652</v>
+        <v>78.396163999999999</v>
       </c>
       <c r="O13" s="8">
         <f t="shared" si="5"/>
-        <v>82.842009250000004</v>
+        <v>83.183286083333329</v>
       </c>
       <c r="P13" s="22">
         <v>13.92</v>
       </c>
-      <c r="Q13" s="77">
+      <c r="Q13" s="79">
+        <v>14.77</v>
+      </c>
+      <c r="R13" s="77">
         <v>14.63</v>
       </c>
-      <c r="R13" s="73">
+      <c r="S13" s="73">
         <v>14.67</v>
       </c>
-      <c r="S13" s="70">
+      <c r="T13" s="70">
         <v>14.7</v>
       </c>
-      <c r="T13" s="67">
+      <c r="U13" s="67">
         <v>14.64</v>
       </c>
-      <c r="U13" s="65">
+      <c r="V13" s="65">
         <v>14.38</v>
       </c>
-      <c r="V13" s="60">
+      <c r="W13" s="60">
         <v>14.31</v>
       </c>
-      <c r="W13" s="58">
+      <c r="X13" s="58">
         <v>14.5</v>
       </c>
-      <c r="X13" s="56">
+      <c r="Y13" s="56">
         <v>14.37</v>
       </c>
-      <c r="Y13" s="54">
+      <c r="Z13" s="54">
         <v>14.2</v>
       </c>
-      <c r="Z13" s="52">
+      <c r="AA13" s="52">
         <v>14.38</v>
       </c>
-      <c r="AA13" s="50">
+      <c r="AB13" s="50">
         <v>14.37</v>
       </c>
-      <c r="AB13" s="47">
+      <c r="AC13" s="47">
         <v>14.78</v>
       </c>
-      <c r="AC13" s="45">
+      <c r="AD13" s="45">
         <v>14.38</v>
       </c>
-      <c r="AD13" s="43">
+      <c r="AE13" s="43">
         <v>14.14</v>
       </c>
-      <c r="AE13" s="40">
+      <c r="AF13" s="40">
         <v>14.5</v>
       </c>
-      <c r="AF13" s="38">
+      <c r="AG13" s="38">
         <v>14.62</v>
       </c>
-      <c r="AG13" s="36">
+      <c r="AH13" s="36">
         <v>15.34</v>
       </c>
-      <c r="AH13" s="31">
+      <c r="AI13" s="31">
         <v>14.27</v>
       </c>
-      <c r="AI13" s="26">
+      <c r="AJ13" s="26">
         <v>14.2</v>
       </c>
-      <c r="AJ13" s="19">
+      <c r="AK13" s="19">
         <v>14.12</v>
       </c>
-      <c r="AK13" s="15">
+      <c r="AL13" s="15">
         <v>14.12</v>
       </c>
-      <c r="AL13" s="10" t="s">
-        <v>40</v>
+      <c r="AM13" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B14" s="25">
         <v>1385</v>
@@ -2707,7 +2763,7 @@
         <v>9.5274000000000001</v>
       </c>
       <c r="D14" s="21">
-        <v>8.31</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E14" s="1">
         <v>-41.55</v>
@@ -2720,7 +2776,7 @@
       </c>
       <c r="H14" s="9">
         <f t="shared" si="0"/>
-        <v>11509.35</v>
+        <v>11495.500000000002</v>
       </c>
       <c r="I14" s="16">
         <f t="shared" si="1"/>
@@ -2728,99 +2784,102 @@
       </c>
       <c r="J14" s="9">
         <f t="shared" si="2"/>
-        <v>-1686.0990000000002</v>
+        <v>-1699.9489999999987</v>
       </c>
       <c r="K14" s="33">
-        <v>45930.660682870373</v>
+        <v>45930.335185185177</v>
       </c>
       <c r="L14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M14" s="8">
         <f t="shared" si="3"/>
-        <v>0.11391625</v>
+        <v>0.11364083333333334</v>
       </c>
       <c r="N14" s="8">
         <f t="shared" si="4"/>
-        <v>153.841645</v>
+        <v>153.65651666666668</v>
       </c>
       <c r="O14" s="8">
         <f t="shared" si="5"/>
-        <v>157.77400624999999</v>
+        <v>157.39255416666668</v>
       </c>
       <c r="P14" s="22">
         <v>16.04</v>
       </c>
-      <c r="Q14" s="77">
+      <c r="Q14" s="79">
+        <v>16.43</v>
+      </c>
+      <c r="R14" s="77">
         <v>16.45</v>
       </c>
-      <c r="R14" s="74">
+      <c r="S14" s="74">
         <v>16.04</v>
       </c>
-      <c r="S14" s="71">
+      <c r="T14" s="71">
         <v>16.04</v>
       </c>
-      <c r="T14" s="66">
+      <c r="U14" s="66">
         <v>15.96</v>
       </c>
-      <c r="U14" s="65">
+      <c r="V14" s="65">
         <v>16.079999999999998</v>
       </c>
-      <c r="V14" s="59">
+      <c r="W14" s="59">
         <v>15.93</v>
       </c>
-      <c r="W14" s="58">
+      <c r="X14" s="58">
         <v>16.079999999999998</v>
       </c>
-      <c r="X14" s="55">
+      <c r="Y14" s="55">
         <v>15.53</v>
       </c>
-      <c r="Y14" s="53">
+      <c r="Z14" s="53">
         <v>15.23</v>
       </c>
-      <c r="Z14" s="52">
+      <c r="AA14" s="52">
         <v>16.190000000000001</v>
       </c>
-      <c r="AA14" s="50">
+      <c r="AB14" s="50">
         <v>16.22</v>
       </c>
-      <c r="AB14" s="47">
+      <c r="AC14" s="47">
         <v>16.41</v>
       </c>
-      <c r="AC14" s="44">
+      <c r="AD14" s="44">
         <v>15.91</v>
       </c>
-      <c r="AD14" s="42">
+      <c r="AE14" s="42">
         <v>15.49</v>
       </c>
-      <c r="AE14" s="41">
+      <c r="AF14" s="41">
         <v>15.93</v>
       </c>
-      <c r="AF14" s="38">
+      <c r="AG14" s="38">
         <v>16.690000000000001</v>
       </c>
-      <c r="AG14" s="36">
+      <c r="AH14" s="36">
         <v>16.350000000000001</v>
       </c>
-      <c r="AH14" s="32">
+      <c r="AI14" s="32">
         <v>14.99</v>
       </c>
-      <c r="AI14" s="27">
+      <c r="AJ14" s="27">
         <v>15.13</v>
       </c>
-      <c r="AJ14" s="18">
+      <c r="AK14" s="18">
         <v>14.82</v>
       </c>
-      <c r="AK14" s="14">
+      <c r="AL14" s="14">
         <v>14.62</v>
       </c>
-      <c r="AL14" s="10" t="s">
-        <v>40</v>
+      <c r="AM14" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" s="25">
         <v>688</v>
@@ -2829,7 +2888,7 @@
         <v>19.151299999999999</v>
       </c>
       <c r="D15" s="21">
-        <v>19.32</v>
+        <v>19.2</v>
       </c>
       <c r="E15" s="1">
         <v>6.88</v>
@@ -2842,7 +2901,7 @@
       </c>
       <c r="H15" s="9">
         <f t="shared" si="0"/>
-        <v>13292.16</v>
+        <v>13209.6</v>
       </c>
       <c r="I15" s="16">
         <f t="shared" si="1"/>
@@ -2850,99 +2909,102 @@
       </c>
       <c r="J15" s="9">
         <f t="shared" si="2"/>
-        <v>116.0655999999999</v>
+        <v>33.505600000000413</v>
       </c>
       <c r="K15" s="33">
-        <v>45902.660682870373</v>
+        <v>45902.335185185177</v>
       </c>
       <c r="L15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M15" s="8">
         <f t="shared" si="3"/>
-        <v>0.22073100000000001</v>
+        <v>0.22111999999999998</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" si="4"/>
-        <v>184.42871999999997</v>
+        <v>183.28319999999999</v>
       </c>
       <c r="O15" s="8">
         <f t="shared" si="5"/>
-        <v>151.86292799999998</v>
+        <v>152.13055999999997</v>
       </c>
       <c r="P15" s="22">
         <v>16.649999999999999</v>
       </c>
-      <c r="Q15" s="76">
+      <c r="Q15" s="78">
+        <v>13.82</v>
+      </c>
+      <c r="R15" s="76">
         <v>13.71</v>
       </c>
-      <c r="R15" s="72">
+      <c r="S15" s="72">
         <v>13.78</v>
       </c>
-      <c r="S15" s="69">
+      <c r="T15" s="69">
         <v>13.85</v>
       </c>
-      <c r="T15" s="66">
+      <c r="U15" s="66">
         <v>13.99</v>
       </c>
-      <c r="U15" s="64">
+      <c r="V15" s="64">
         <v>13.93</v>
       </c>
-      <c r="V15" s="59">
+      <c r="W15" s="59">
         <v>13.89</v>
       </c>
-      <c r="W15" s="57">
+      <c r="X15" s="57">
         <v>14.05</v>
       </c>
-      <c r="X15" s="55">
+      <c r="Y15" s="55">
         <v>14.2</v>
       </c>
-      <c r="Y15" s="53">
+      <c r="Z15" s="53">
         <v>14.07</v>
       </c>
-      <c r="Z15" s="51">
+      <c r="AA15" s="51">
         <v>14.03</v>
       </c>
-      <c r="AA15" s="49">
+      <c r="AB15" s="49">
         <v>14.07</v>
       </c>
-      <c r="AB15" s="46">
+      <c r="AC15" s="46">
         <v>14.41</v>
       </c>
-      <c r="AC15" s="44">
+      <c r="AD15" s="44">
         <v>13.98</v>
       </c>
-      <c r="AD15" s="42">
+      <c r="AE15" s="42">
         <v>14.21</v>
       </c>
-      <c r="AE15" s="41">
+      <c r="AF15" s="41">
         <v>14.44</v>
       </c>
-      <c r="AF15" s="39">
+      <c r="AG15" s="39">
         <v>14.93</v>
       </c>
-      <c r="AG15" s="37">
+      <c r="AH15" s="37">
         <v>14.89</v>
       </c>
-      <c r="AH15" s="32">
+      <c r="AI15" s="32">
         <v>13.42</v>
       </c>
-      <c r="AI15" s="26">
+      <c r="AJ15" s="26">
         <v>16.649999999999999</v>
       </c>
-      <c r="AJ15" s="19">
+      <c r="AK15" s="19">
         <v>16.649999999999999</v>
       </c>
-      <c r="AK15" s="15">
+      <c r="AL15" s="15">
         <v>16.649999999999999</v>
       </c>
-      <c r="AL15" s="10" t="s">
-        <v>40</v>
+      <c r="AM15" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" s="25">
         <v>276</v>
@@ -2951,7 +3013,7 @@
         <v>38.83</v>
       </c>
       <c r="D16" s="21">
-        <v>35.520000000000003</v>
+        <v>35.47</v>
       </c>
       <c r="E16" s="1">
         <v>-72.239999999999995</v>
@@ -2964,7 +3026,7 @@
       </c>
       <c r="H16" s="9">
         <f t="shared" si="0"/>
-        <v>9803.52</v>
+        <v>9789.7199999999993</v>
       </c>
       <c r="I16" s="16">
         <f t="shared" si="1"/>
@@ -2972,99 +3034,102 @@
       </c>
       <c r="J16" s="9">
         <f t="shared" si="2"/>
-        <v>-913.55999999999949</v>
+        <v>-927.36000000000058</v>
       </c>
       <c r="K16" s="33">
-        <v>45877.660682870373</v>
+        <v>45884.335185185177</v>
       </c>
       <c r="L16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M16" s="8">
         <f t="shared" si="3"/>
-        <v>0.24094400000000002</v>
+        <v>0.23203291666666662</v>
       </c>
       <c r="N16" s="8">
         <f t="shared" si="4"/>
-        <v>56.533632000000004</v>
+        <v>56.45405199999999</v>
       </c>
       <c r="O16" s="8">
         <f t="shared" si="5"/>
-        <v>66.500544000000005</v>
+        <v>64.041084999999995</v>
       </c>
       <c r="P16" s="30">
         <v>6.92</v>
       </c>
-      <c r="Q16" s="77">
+      <c r="Q16" s="79">
+        <v>7.85</v>
+      </c>
+      <c r="R16" s="77">
         <v>8.14</v>
       </c>
-      <c r="R16" s="72">
+      <c r="S16" s="72">
         <v>8.08</v>
       </c>
-      <c r="S16" s="69">
+      <c r="T16" s="69">
         <v>8</v>
       </c>
-      <c r="T16" s="67">
+      <c r="U16" s="67">
         <v>32.4</v>
       </c>
-      <c r="U16" s="65">
+      <c r="V16" s="65">
         <v>8.08</v>
       </c>
-      <c r="V16" s="60">
+      <c r="W16" s="60">
         <v>7.82</v>
       </c>
-      <c r="W16" s="58">
+      <c r="X16" s="58">
         <v>8.43</v>
       </c>
-      <c r="X16" s="56">
+      <c r="Y16" s="56">
         <v>7.18</v>
       </c>
-      <c r="Y16" s="53">
+      <c r="Z16" s="53">
         <v>5.05</v>
       </c>
-      <c r="Z16" s="52">
+      <c r="AA16" s="52">
         <v>7.3</v>
       </c>
-      <c r="AA16" s="50">
+      <c r="AB16" s="50">
         <v>7.54</v>
       </c>
-      <c r="AB16" s="46">
+      <c r="AC16" s="46">
         <v>6.11</v>
       </c>
-      <c r="AC16" s="45">
+      <c r="AD16" s="45">
         <v>11.39</v>
       </c>
-      <c r="AD16" s="43">
+      <c r="AE16" s="43">
         <v>8.17</v>
       </c>
-      <c r="AE16" s="40">
+      <c r="AF16" s="40">
         <v>9.17</v>
       </c>
-      <c r="AF16" s="38">
+      <c r="AG16" s="38">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AG16" s="36">
+      <c r="AH16" s="36">
         <v>7.08</v>
       </c>
-      <c r="AH16" s="31">
+      <c r="AI16" s="31">
         <v>9.1300000000000008</v>
       </c>
-      <c r="AI16" s="17">
+      <c r="AJ16" s="17">
         <v>7.92</v>
       </c>
-      <c r="AJ16" s="17">
+      <c r="AK16" s="17">
         <v>9.2899999999999991</v>
       </c>
-      <c r="AK16" s="17">
+      <c r="AL16" s="17">
         <v>8.0399999999999991</v>
       </c>
-      <c r="AL16" s="10" t="s">
-        <v>40</v>
+      <c r="AM16" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B17" s="25">
         <v>350</v>
@@ -3073,7 +3138,7 @@
         <v>17.920000000000002</v>
       </c>
       <c r="D17" s="21">
-        <v>16.89</v>
+        <v>16.84</v>
       </c>
       <c r="E17" s="1">
         <v>-24.5</v>
@@ -3086,7 +3151,7 @@
       </c>
       <c r="H17" s="9">
         <f t="shared" si="0"/>
-        <v>5911.5</v>
+        <v>5894</v>
       </c>
       <c r="I17" s="16">
         <f t="shared" si="1"/>
@@ -3094,99 +3159,102 @@
       </c>
       <c r="J17" s="9">
         <f t="shared" si="2"/>
-        <v>-360.50000000000091</v>
+        <v>-378.00000000000091</v>
       </c>
       <c r="K17" s="33">
-        <v>45866.660694444443</v>
+        <v>45866.335185185177</v>
       </c>
       <c r="L17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M17" s="8">
         <f t="shared" si="3"/>
-        <v>0.173404</v>
+        <v>0.17204866666666666</v>
       </c>
       <c r="N17" s="8">
         <f t="shared" si="4"/>
-        <v>60.986975000000001</v>
+        <v>60.806433333333338</v>
       </c>
       <c r="O17" s="8">
         <f t="shared" si="5"/>
-        <v>60.691400000000009</v>
+        <v>60.21703333333334</v>
       </c>
       <c r="P17" s="22">
         <v>12.38</v>
       </c>
-      <c r="Q17" s="76">
+      <c r="Q17" s="78">
+        <v>12.26</v>
+      </c>
+      <c r="R17" s="76">
         <v>12.32</v>
       </c>
-      <c r="R17" s="73">
+      <c r="S17" s="73">
         <v>12.39</v>
       </c>
-      <c r="S17" s="70">
+      <c r="T17" s="70">
         <v>12.39</v>
       </c>
-      <c r="T17" s="67">
+      <c r="U17" s="67">
         <v>12.44</v>
       </c>
-      <c r="U17" s="65">
+      <c r="V17" s="65">
         <v>12.45</v>
       </c>
-      <c r="V17" s="60">
+      <c r="W17" s="60">
         <v>12.49</v>
       </c>
-      <c r="W17" s="58">
+      <c r="X17" s="58">
         <v>12.53</v>
       </c>
-      <c r="X17" s="56">
+      <c r="Y17" s="56">
         <v>12.57</v>
       </c>
-      <c r="Y17" s="54">
+      <c r="Z17" s="54">
         <v>12.57</v>
       </c>
-      <c r="Z17" s="52">
+      <c r="AA17" s="52">
         <v>12.69</v>
       </c>
-      <c r="AA17" s="50">
+      <c r="AB17" s="50">
         <v>12.72</v>
       </c>
-      <c r="AB17" s="48">
+      <c r="AC17" s="48">
         <v>12.91</v>
       </c>
-      <c r="AC17" s="45">
+      <c r="AD17" s="45">
         <v>12.75</v>
       </c>
-      <c r="AD17" s="43">
+      <c r="AE17" s="43">
         <v>12.79</v>
       </c>
-      <c r="AE17" s="40">
+      <c r="AF17" s="40">
         <v>12.91</v>
       </c>
-      <c r="AF17" s="38">
+      <c r="AG17" s="38">
         <v>13.15</v>
       </c>
-      <c r="AG17" s="36">
+      <c r="AH17" s="36">
         <v>13.14</v>
       </c>
-      <c r="AH17" s="31">
+      <c r="AI17" s="31">
         <v>13.02</v>
       </c>
-      <c r="AI17" s="26">
+      <c r="AJ17" s="26">
         <v>12.68</v>
       </c>
-      <c r="AJ17" s="24">
+      <c r="AK17" s="24">
         <v>12.68</v>
       </c>
-      <c r="AK17" s="15">
+      <c r="AL17" s="15">
         <v>12.68</v>
       </c>
-      <c r="AL17" s="10" t="s">
-        <v>40</v>
+      <c r="AM17" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="25">
         <v>579</v>
@@ -3195,7 +3263,7 @@
         <v>16.540700000000001</v>
       </c>
       <c r="D18" s="21">
-        <v>14.8</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1">
         <v>-28.95</v>
@@ -3208,7 +3276,7 @@
       </c>
       <c r="H18" s="9">
         <f t="shared" si="0"/>
-        <v>8569.2000000000007</v>
+        <v>8685</v>
       </c>
       <c r="I18" s="16">
         <f t="shared" si="1"/>
@@ -3216,99 +3284,102 @@
       </c>
       <c r="J18" s="9">
         <f t="shared" si="2"/>
-        <v>-1007.8652999999995</v>
+        <v>-892.06530000000021</v>
       </c>
       <c r="K18" s="33">
-        <v>45866.660694444443</v>
+        <v>45866.335185185177</v>
       </c>
       <c r="L18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M18" s="8">
         <f t="shared" si="3"/>
-        <v>0.15823666666666666</v>
+        <v>0.1565</v>
       </c>
       <c r="N18" s="8">
         <f t="shared" si="4"/>
-        <v>84.763670000000005</v>
+        <v>85.909125000000003</v>
       </c>
       <c r="O18" s="8">
         <f t="shared" si="5"/>
-        <v>91.619030000000009</v>
+        <v>90.613500000000002</v>
       </c>
       <c r="P18" s="22">
         <v>11.87</v>
       </c>
-      <c r="Q18" s="77">
+      <c r="Q18" s="79">
+        <v>12.52</v>
+      </c>
+      <c r="R18" s="77">
         <v>12.83</v>
       </c>
-      <c r="R18" s="73">
+      <c r="S18" s="73">
         <v>12.89</v>
       </c>
-      <c r="S18" s="70">
+      <c r="T18" s="70">
         <v>12.77</v>
       </c>
-      <c r="T18" s="67">
+      <c r="U18" s="67">
         <v>12.66</v>
       </c>
-      <c r="U18" s="65">
+      <c r="V18" s="65">
         <v>12.67</v>
       </c>
-      <c r="V18" s="60">
+      <c r="W18" s="60">
         <v>12.74</v>
       </c>
-      <c r="W18" s="58">
+      <c r="X18" s="58">
         <v>12.81</v>
       </c>
-      <c r="X18" s="56">
+      <c r="Y18" s="56">
         <v>12.89</v>
       </c>
-      <c r="Y18" s="54">
+      <c r="Z18" s="54">
         <v>12.92</v>
       </c>
-      <c r="Z18" s="52">
+      <c r="AA18" s="52">
         <v>13.1</v>
       </c>
-      <c r="AA18" s="50">
+      <c r="AB18" s="50">
         <v>13.2</v>
       </c>
-      <c r="AB18" s="47">
+      <c r="AC18" s="47">
         <v>13.39</v>
       </c>
-      <c r="AC18" s="45">
+      <c r="AD18" s="45">
         <v>13.25</v>
       </c>
-      <c r="AD18" s="43">
+      <c r="AE18" s="43">
         <v>13.33</v>
       </c>
-      <c r="AE18" s="40">
+      <c r="AF18" s="40">
         <v>13.36</v>
       </c>
-      <c r="AF18" s="38">
+      <c r="AG18" s="38">
         <v>13.79</v>
       </c>
-      <c r="AG18" s="36">
+      <c r="AH18" s="36">
         <v>14.02</v>
       </c>
-      <c r="AH18" s="31">
+      <c r="AI18" s="31">
         <v>13.48</v>
       </c>
-      <c r="AI18" s="26">
+      <c r="AJ18" s="26">
         <v>12.28</v>
       </c>
-      <c r="AJ18" s="19">
+      <c r="AK18" s="19">
         <v>12.28</v>
       </c>
-      <c r="AK18" s="15">
+      <c r="AL18" s="15">
         <v>12.28</v>
       </c>
-      <c r="AL18" s="10" t="s">
-        <v>40</v>
+      <c r="AM18" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="25">
         <v>552</v>
@@ -3317,7 +3388,7 @@
         <v>22.328800000000001</v>
       </c>
       <c r="D19" s="21">
-        <v>17.03</v>
+        <v>17.3</v>
       </c>
       <c r="E19" s="1">
         <v>-143.52000000000001</v>
@@ -3330,7 +3401,7 @@
       </c>
       <c r="H19" s="9">
         <f t="shared" si="0"/>
-        <v>9400.5600000000013</v>
+        <v>9549.6</v>
       </c>
       <c r="I19" s="16">
         <f t="shared" si="1"/>
@@ -3338,99 +3409,102 @@
       </c>
       <c r="J19" s="9">
         <f t="shared" si="2"/>
-        <v>-2924.9375999999993</v>
+        <v>-2775.8976000000002</v>
       </c>
       <c r="K19" s="33">
-        <v>45869.660694444443</v>
+        <v>45869.335196759261</v>
       </c>
       <c r="L19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M19" s="8">
         <f t="shared" si="3"/>
-        <v>0.28354950000000001</v>
+        <v>0.27838583333333333</v>
       </c>
       <c r="N19" s="8">
         <f t="shared" si="4"/>
-        <v>127.612602</v>
+        <v>129.63582</v>
       </c>
       <c r="O19" s="8">
         <f t="shared" si="5"/>
-        <v>156.51932400000001</v>
+        <v>153.66898</v>
       </c>
       <c r="P19" s="22">
         <v>16.29</v>
       </c>
-      <c r="Q19" s="77">
+      <c r="Q19" s="79">
+        <v>19.309999999999999</v>
+      </c>
+      <c r="R19" s="77">
         <v>19.98</v>
       </c>
-      <c r="R19" s="73">
+      <c r="S19" s="73">
         <v>20.010000000000002</v>
       </c>
-      <c r="S19" s="70">
+      <c r="T19" s="70">
         <v>19.29</v>
       </c>
-      <c r="T19" s="67">
+      <c r="U19" s="67">
         <v>19.37</v>
       </c>
-      <c r="U19" s="65">
+      <c r="V19" s="65">
         <v>18.52</v>
       </c>
-      <c r="V19" s="60">
+      <c r="W19" s="60">
         <v>18.350000000000001</v>
       </c>
-      <c r="W19" s="58">
+      <c r="X19" s="58">
         <v>19.190000000000001</v>
       </c>
-      <c r="X19" s="56">
+      <c r="Y19" s="56">
         <v>20</v>
       </c>
-      <c r="Y19" s="54">
+      <c r="Z19" s="54">
         <v>18.940000000000001</v>
       </c>
-      <c r="Z19" s="52">
+      <c r="AA19" s="52">
         <v>19.29</v>
       </c>
-      <c r="AA19" s="50">
+      <c r="AB19" s="50">
         <v>19.260000000000002</v>
       </c>
-      <c r="AB19" s="47">
+      <c r="AC19" s="47">
         <v>18.559999999999999</v>
       </c>
-      <c r="AC19" s="45">
+      <c r="AD19" s="45">
         <v>20.56</v>
       </c>
-      <c r="AD19" s="43">
+      <c r="AE19" s="43">
         <v>20.309999999999999</v>
       </c>
-      <c r="AE19" s="40">
+      <c r="AF19" s="40">
         <v>20.75</v>
       </c>
-      <c r="AF19" s="38">
+      <c r="AG19" s="38">
         <v>21.94</v>
       </c>
-      <c r="AG19" s="36">
+      <c r="AH19" s="36">
         <v>22.22</v>
       </c>
-      <c r="AH19" s="31">
+      <c r="AI19" s="31">
         <v>19.760000000000002</v>
       </c>
-      <c r="AI19" s="26">
+      <c r="AJ19" s="26">
         <v>16.649999999999999</v>
       </c>
-      <c r="AJ19" s="19">
+      <c r="AK19" s="19">
         <v>16.649999999999999</v>
       </c>
-      <c r="AK19" s="15">
+      <c r="AL19" s="15">
         <v>16.649999999999999</v>
       </c>
-      <c r="AL19" s="10" t="s">
-        <v>40</v>
+      <c r="AM19" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="25">
         <v>125</v>
@@ -3439,7 +3513,7 @@
         <v>11.91</v>
       </c>
       <c r="D20" s="21">
-        <v>12.42</v>
+        <v>12.58</v>
       </c>
       <c r="E20" s="21">
         <v>78.099999999999994</v>
@@ -3452,7 +3526,7 @@
       </c>
       <c r="H20" s="9">
         <f t="shared" si="0"/>
-        <v>1552.5</v>
+        <v>1572.5</v>
       </c>
       <c r="I20" s="16">
         <f t="shared" si="1"/>
@@ -3460,42 +3534,42 @@
       </c>
       <c r="J20" s="9">
         <f t="shared" si="2"/>
-        <v>63.75</v>
+        <v>83.75</v>
       </c>
       <c r="K20" s="33">
-        <v>45870.660694444443</v>
+        <v>45902.335196759261</v>
       </c>
       <c r="L20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M20" s="8">
         <v>0.17</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" si="4"/>
-        <v>20.557687500000004</v>
+        <v>20.822520833333336</v>
       </c>
       <c r="O20" s="8">
         <f t="shared" si="5"/>
-        <v>21.411562500000002</v>
+        <v>21.268062499999999</v>
       </c>
       <c r="P20" s="22">
         <v>15.89</v>
       </c>
-      <c r="Q20" s="77">
+      <c r="Q20" s="79">
+        <v>16.23</v>
+      </c>
+      <c r="R20" s="77">
         <v>16.55</v>
       </c>
-      <c r="R20" s="73">
+      <c r="S20" s="73">
         <v>16.399999999999999</v>
       </c>
-      <c r="S20" s="70">
+      <c r="T20" s="70">
         <v>16</v>
       </c>
-      <c r="T20" s="67">
+      <c r="U20" s="67">
         <v>16.22</v>
-      </c>
-      <c r="U20" s="22">
-        <v>15.89</v>
       </c>
       <c r="V20" s="22">
         <v>15.89</v>
@@ -3545,13 +3619,16 @@
       <c r="AK20" s="22">
         <v>15.89</v>
       </c>
-      <c r="AL20" s="10" t="s">
-        <v>60</v>
+      <c r="AL20" s="22">
+        <v>15.89</v>
+      </c>
+      <c r="AM20" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B21" s="25">
         <v>1060</v>
@@ -3560,7 +3637,7 @@
         <v>9.42</v>
       </c>
       <c r="D21" s="22">
-        <v>9.4499999999999993</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="E21" s="21">
         <v>-180.2</v>
@@ -3573,7 +3650,7 @@
       </c>
       <c r="H21" s="9">
         <f t="shared" si="0"/>
-        <v>10017</v>
+        <v>10207.800000000001</v>
       </c>
       <c r="I21" s="16">
         <f t="shared" si="1"/>
@@ -3581,45 +3658,45 @@
       </c>
       <c r="J21" s="9">
         <f t="shared" si="2"/>
-        <v>31.799999999999272</v>
+        <v>222.60000000000036</v>
       </c>
       <c r="K21" s="33">
-        <v>45910.660694444443</v>
+        <v>45910.335196759261</v>
       </c>
       <c r="L21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M21" s="62">
         <v>0.12</v>
       </c>
       <c r="N21" s="8">
         <f t="shared" si="4"/>
-        <v>128.38455000000002</v>
+        <v>130.82997000000003</v>
       </c>
       <c r="O21" s="8">
         <f t="shared" si="5"/>
-        <v>127.71674999999999</v>
+        <v>127.42737000000004</v>
       </c>
       <c r="P21" s="63">
         <v>15.38</v>
       </c>
-      <c r="Q21" s="76">
+      <c r="Q21" s="78">
+        <v>14.98</v>
+      </c>
+      <c r="R21" s="76">
         <v>15.3</v>
       </c>
-      <c r="R21" s="72">
+      <c r="S21" s="72">
         <v>15.27</v>
       </c>
-      <c r="S21" s="69">
+      <c r="T21" s="69">
         <v>14.83</v>
       </c>
-      <c r="T21" s="67">
+      <c r="U21" s="67">
         <v>15.52</v>
       </c>
-      <c r="U21" s="64">
+      <c r="V21" s="64">
         <v>15.24</v>
-      </c>
-      <c r="V21" s="63">
-        <v>15.38</v>
       </c>
       <c r="W21" s="63">
         <v>15.38</v>
@@ -3666,13 +3743,16 @@
       <c r="AK21" s="63">
         <v>15.38</v>
       </c>
-      <c r="AL21" t="s">
-        <v>61</v>
+      <c r="AL21" s="63">
+        <v>15.38</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" s="25">
         <v>285</v>
@@ -3681,7 +3761,7 @@
         <v>35.299999999999997</v>
       </c>
       <c r="D22" s="22">
-        <v>35.520000000000003</v>
+        <v>35.47</v>
       </c>
       <c r="E22" s="21">
         <v>17.100000000000001</v>
@@ -3694,7 +3774,7 @@
       </c>
       <c r="H22" s="9">
         <f t="shared" si="0"/>
-        <v>10123.200000000001</v>
+        <v>10108.949999999999</v>
       </c>
       <c r="I22" s="16">
         <f t="shared" si="1"/>
@@ -3702,42 +3782,42 @@
       </c>
       <c r="J22" s="9">
         <f t="shared" si="2"/>
-        <v>62.700000000000728</v>
+        <v>48.449999999998909</v>
       </c>
       <c r="K22" s="68">
-        <v>45877.660694444443</v>
+        <v>45884.335196759261</v>
       </c>
       <c r="L22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M22">
         <v>0.24</v>
       </c>
       <c r="N22" s="8">
         <f t="shared" si="4"/>
-        <v>68.162880000000001</v>
+        <v>68.066929999999999</v>
       </c>
       <c r="O22" s="8">
         <f t="shared" si="5"/>
-        <v>68.66904000000001</v>
+        <v>66.129381249999994</v>
       </c>
       <c r="P22" s="13">
         <v>8.08</v>
       </c>
-      <c r="Q22" s="77">
+      <c r="Q22" s="78">
+        <v>7.85</v>
+      </c>
+      <c r="R22" s="77">
         <v>8.14</v>
       </c>
-      <c r="R22" s="72">
+      <c r="S22" s="72">
         <v>8.08</v>
       </c>
-      <c r="S22" s="69">
+      <c r="T22" s="69">
         <v>8</v>
       </c>
-      <c r="T22" s="67">
+      <c r="U22" s="67">
         <v>32.4</v>
-      </c>
-      <c r="U22" s="13">
-        <v>8.08</v>
       </c>
       <c r="V22" s="13">
         <v>8.08</v>
@@ -3787,13 +3867,16 @@
       <c r="AK22" s="13">
         <v>8.08</v>
       </c>
-      <c r="AL22" t="s">
-        <v>61</v>
+      <c r="AL22" s="13">
+        <v>8.08</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" s="25">
         <v>1330</v>
@@ -3802,7 +3885,7 @@
         <v>7.43</v>
       </c>
       <c r="D23" s="22">
-        <v>6.23</v>
+        <v>6.71</v>
       </c>
       <c r="E23">
         <v>33.25</v>
@@ -3815,7 +3898,7 @@
       </c>
       <c r="H23" s="9">
         <f t="shared" si="0"/>
-        <v>8285.9000000000015</v>
+        <v>8924.2999999999993</v>
       </c>
       <c r="I23" s="16">
         <f t="shared" si="1"/>
@@ -3823,42 +3906,42 @@
       </c>
       <c r="J23" s="9">
         <f t="shared" si="2"/>
-        <v>-1595.9999999999982</v>
+        <v>-957.60000000000036</v>
       </c>
       <c r="K23" s="68">
-        <v>45898.66070601852</v>
+        <v>45930.335196759261</v>
       </c>
       <c r="L23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M23">
         <v>0.14000000000000001</v>
       </c>
       <c r="N23" s="8">
         <f t="shared" si="4"/>
-        <v>151.42482250000003</v>
+        <v>163.09158249999999</v>
       </c>
       <c r="O23" s="8">
         <f t="shared" si="5"/>
-        <v>180.97786583333337</v>
+        <v>187.6334075</v>
       </c>
       <c r="P23" s="13">
         <v>21.93</v>
       </c>
-      <c r="Q23" s="77">
+      <c r="Q23" s="79">
+        <v>25.23</v>
+      </c>
+      <c r="R23" s="77">
         <v>26.21</v>
       </c>
-      <c r="R23" s="73">
+      <c r="S23" s="73">
         <v>24.42</v>
       </c>
-      <c r="S23" s="70">
+      <c r="T23" s="70">
         <v>24.31</v>
       </c>
-      <c r="T23" s="67">
+      <c r="U23" s="67">
         <v>22.67</v>
-      </c>
-      <c r="U23" s="13">
-        <v>21.93</v>
       </c>
       <c r="V23" s="13">
         <v>21.93</v>
@@ -3908,108 +3991,115 @@
       <c r="AK23" s="13">
         <v>21.93</v>
       </c>
-      <c r="AL23" t="s">
-        <v>61</v>
+      <c r="AL23" s="13">
+        <v>21.93</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M25" s="34">
         <f>AVERAGE(M3:M23)</f>
-        <v>0.18159304365079365</v>
+        <v>0.18096572619047618</v>
       </c>
       <c r="N25" s="34">
         <f>SUM(N3:N23)</f>
-        <v>2209.8638929166664</v>
+        <v>2249.7165606666672</v>
       </c>
       <c r="O25" s="35">
         <f>SUM(O3:O23)</f>
-        <v>2293.8843441666668</v>
+        <v>2295.4421065000001</v>
       </c>
       <c r="P25" s="35">
         <f>AVERAGE(P3:P24)</f>
         <v>16.278571428571428</v>
       </c>
       <c r="Q25" s="35">
-        <f t="shared" ref="Q25:AK25" si="6">AVERAGE(Q3:Q24)</f>
-        <v>17.084761904761905</v>
+        <f t="shared" ref="Q25:AL25" si="6">AVERAGE(Q3:Q24)</f>
+        <v>16.730952380952381</v>
       </c>
       <c r="R25" s="35">
         <f t="shared" si="6"/>
-        <v>16.897142857142853</v>
+        <v>17.084761904761905</v>
       </c>
       <c r="S25" s="35">
         <f t="shared" si="6"/>
-        <v>16.725714285714282</v>
+        <v>16.897142857142853</v>
       </c>
       <c r="T25" s="35">
         <f t="shared" si="6"/>
-        <v>18.940000000000005</v>
+        <v>16.725714285714282</v>
       </c>
       <c r="U25" s="35">
         <f t="shared" si="6"/>
-        <v>16.454761904761902</v>
+        <v>18.940000000000005</v>
       </c>
       <c r="V25" s="35">
         <f t="shared" si="6"/>
-        <v>16.526666666666667</v>
+        <v>16.454761904761902</v>
       </c>
       <c r="W25" s="35">
         <f t="shared" si="6"/>
-        <v>16.744285714285713</v>
+        <v>16.526666666666667</v>
       </c>
       <c r="X25" s="35">
         <f t="shared" si="6"/>
-        <v>16.857619047619046</v>
+        <v>16.744285714285713</v>
       </c>
       <c r="Y25" s="35">
         <f t="shared" si="6"/>
-        <v>16.507619047619045</v>
+        <v>16.857619047619046</v>
       </c>
       <c r="Z25" s="35">
         <f t="shared" si="6"/>
-        <v>16.923809523809524</v>
+        <v>16.507619047619045</v>
       </c>
       <c r="AA25" s="35">
         <f t="shared" si="6"/>
-        <v>16.900476190476191</v>
+        <v>16.923809523809524</v>
       </c>
       <c r="AB25" s="35">
         <f t="shared" si="6"/>
-        <v>17.042857142857141</v>
+        <v>16.900476190476191</v>
       </c>
       <c r="AC25" s="35">
         <f t="shared" si="6"/>
-        <v>17.389047619047616</v>
+        <v>17.042857142857141</v>
       </c>
       <c r="AD25" s="35">
         <f t="shared" si="6"/>
-        <v>17.47190476190476</v>
+        <v>17.389047619047616</v>
       </c>
       <c r="AE25" s="35">
         <f t="shared" si="6"/>
-        <v>18.075238095238099</v>
+        <v>17.47190476190476</v>
       </c>
       <c r="AF25" s="35">
         <f t="shared" si="6"/>
-        <v>18.781428571428574</v>
+        <v>18.075238095238099</v>
       </c>
       <c r="AG25" s="35">
         <f t="shared" si="6"/>
-        <v>19.168571428571422</v>
+        <v>18.781428571428574</v>
       </c>
       <c r="AH25" s="35">
         <f t="shared" si="6"/>
-        <v>17.930476190476192</v>
+        <v>19.168571428571422</v>
       </c>
       <c r="AI25" s="35">
         <f t="shared" si="6"/>
-        <v>17.470476190476187</v>
+        <v>17.930476190476192</v>
       </c>
       <c r="AJ25" s="35">
         <f t="shared" si="6"/>
+        <v>17.470476190476187</v>
+      </c>
+      <c r="AK25" s="35">
+        <f t="shared" si="6"/>
         <v>17.38428571428571</v>
       </c>
-      <c r="AK25" s="35">
+      <c r="AL25" s="35">
         <f t="shared" si="6"/>
         <v>17.251428571428569</v>
       </c>

</xml_diff>